<commit_message>
SUCCESS - counts and add context information to match
</commit_message>
<xml_diff>
--- a/Output/Electronic Copy Counts for - All Hirsh Reserves - 06-04-2020.xlsx
+++ b/Output/Electronic Copy Counts for - All Hirsh Reserves - 06-04-2020.xlsx
@@ -678,7 +678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -693,77 +693,176 @@
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>MMS Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Title (Normalized)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Course Code</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Course Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MMS ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Processing Department</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>URL or Collection</t>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Author (contributor)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bibliographic Level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Resource Type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Match MMS ID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Match Title</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Match Author</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Match Publication Year</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Match URL or Collection</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>991017473844303851</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>management principles for health professionals</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>2202-20859</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0216-01-Management Planning</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[2017]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Liebler, Joan Gratto, author.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>McConnell, Charles R., author.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>991017467548503851</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>management principles for health professionals</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>liebler, joan gratto, author.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Individually Purchased eBooks</t>
         </is>
@@ -780,7 +879,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,77 +894,176 @@
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>MMS Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Title (Normalized)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Course Code</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Course Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MMS ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Processing Department</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>URL or Collection</t>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Author (contributor)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bibliographic Level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Resource Type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Match MMS ID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Match Title</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Match Author</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Match Publication Year</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Match URL or Collection</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>991005267559703851</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>focus groups a practical guide for applied research</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>2202-20857</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[2015]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Krueger, Richard A.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Casey, Mary Anne (Mary Anne W.)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>991012436609703851</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>focus groups a practical guide for applied research</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>krueger, richard a.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>HathiTrust (free during Covid-19)</t>
         </is>
@@ -874,27 +1072,68 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>991013153629703851</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>scale development theory and applications</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>2202-20857</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>c2012.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>DeVellis, Robert F.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>991001524649703851</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>scale development theory and applications</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
         <is>
           <t>HathiTrust (free during Covid-19)</t>
         </is>
@@ -903,35 +1142,80 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>991003181969703851</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>management principles for health professionals</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>2202-20859</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0216-01-Management Planning</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>c2008.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Liebler, Joan Gratto.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>McConnell, Charles R.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>991003081379703851</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>management principles for health professionals</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>liebler, joan gratto.</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>2004</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>Individually Purchased eBooks</t>
         </is>
@@ -940,35 +1224,76 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>991017473845203851</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>management control in nonprofit organizations</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>2202-20859</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0216-01-Management Planning</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>©2016.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Young, David W.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>991015153869703851</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>management control in nonprofit organizations</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>young, david w.</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>2012</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>HathiTrust (free during Covid-19)</t>
         </is>
@@ -1050,212 +1375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Course Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Course Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MMS ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Author</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>URL or Collection</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2202-20857</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>991012436609703851</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>focus groups a practical guide for applied research</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>krueger, richard a.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>HathiTrust (free during Covid-19)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2202-20857</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>991001524649703851</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>scale development theory and applications</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>HathiTrust (free during Covid-19)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2202-20859</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Sp20-NUTR-0216-01-Management Planning</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>991003081379703851</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>management principles for health professionals</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>liebler, joan gratto.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2004</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Individually Purchased eBooks</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2202-20859</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Sp20-NUTR-0216-01-Management Planning</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>991015153869703851</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>management control in nonprofit organizations</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>young, david w.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>HathiTrust (free during Covid-19)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1274,68 +1394,569 @@
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MMS ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Year</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>URL or Collection</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Author (contributor)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bibliographic Level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>MMS Id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Match Author</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Match MMS ID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Match Publication Year</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Match Title</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Match URL or Collection</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Processing Department</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Date</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Resource Type</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Title (Normalized)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Course Code</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Course Name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Processing Department</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Date</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Author</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Author (contributor)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Bibliographic Level</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Resource Type</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Semester</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>2202-20857</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Krueger, Richard A.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Casey, Mary Anne (Mary Anne W.)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>991005267559703851</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>krueger, richard a.</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>991012436609703851</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>focus groups a practical guide for applied research</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>HathiTrust (free during Covid-19)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>[2015]</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>focus groups a practical guide for applied research</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2202-20857</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>DeVellis, Robert F.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>991013153629703851</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>991001524649703851</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>scale development theory and applications</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>HathiTrust (free during Covid-19)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>c2012.</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>scale development theory and applications</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2202-20859</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sp20-NUTR-0216-01-Management Planning</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Liebler, Joan Gratto.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>McConnell, Charles R.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>991003181969703851</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>liebler, joan gratto.</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>991003081379703851</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>management principles for health professionals</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Individually Purchased eBooks</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>c2008.</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>management principles for health professionals</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2202-20859</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sp20-NUTR-0216-01-Management Planning</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Young, David W.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>991017473845203851</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>young, david w.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>991015153869703851</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>management control in nonprofit organizations</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>HathiTrust (free during Covid-19)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>©2016.</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>management control in nonprofit organizations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MMS Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Title (Normalized)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Processing Department</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Author (contributor)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bibliographic Level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Resource Type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Match MMS ID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Match Title</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Match Author</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Match Publication Year</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Match URL or Collection</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>991002905429703851</t>
         </is>
       </c>
@@ -1385,6 +2006,31 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>991003179379703851</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>advanced male urethral and genital reconstructive surgery</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>brandes, steven b., editor.</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>http://link.springer.com/10.1007/978-1-4614-7708-2|Springer English/International eBooks</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1438,6 +2084,31 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>991009906229703851</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>the practice of social research</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>babbie, earl r.</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1979</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>HathiTrust (free during Covid-19)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1495,6 +2166,27 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>991003245689703851</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>asking questions the definitive guide to questionnaire design for market research political polls and social and health questionnaires</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>bradburn, norman m.</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1552,6 +2244,31 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>991017862649703851</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>internet phone mail and mixedmode surveys the tailored design method</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>dillman, don a., 1941-</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Individually Purchased eBooks</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1605,6 +2322,31 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>991009521169703851</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>designing household survey questionnaires for developing countries  lessons from 15 years of the living standards measurement study</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>grosh, margaret e.</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>HathiTrust (free during Covid-19)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1662,6 +2404,27 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>991017843948603851</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>realworld evaluation working under budget time data and political constraints</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>bamberger, michael.</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1715,6 +2478,27 @@
           <t>2202</t>
         </is>
       </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>991017843948603851</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>realworld evaluation working under budget time data and political constraints</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>bamberger, michael.</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix electronic books on course matching
</commit_message>
<xml_diff>
--- a/Output/Electronic Copy Counts for - All Hirsh Reserves - 06-04-2020.xlsx
+++ b/Output/Electronic Copy Counts for - All Hirsh Reserves - 06-04-2020.xlsx
@@ -614,13 +614,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -879,7 +879,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>991001524649703851</t>
+          <t>991001730479703851</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -1131,8 +1131,16 @@
           <t>scale development theory and applications</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>devellis, robert f.</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>2003</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr">
         <is>
           <t>HathiTrust (free during Covid-19)</t>
@@ -1142,12 +1150,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>991003181969703851</t>
+          <t>991017473845203851</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>management principles for health professionals</t>
+          <t>management control in nonprofit organizations</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1167,19 +1175,15 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>c2008.</t>
+          <t>©2016.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Liebler, Joan Gratto.</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>McConnell, Charles R.</t>
-        </is>
-      </c>
+          <t>Young, David W.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>m</t>
@@ -1197,103 +1201,25 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>991003081379703851</t>
+          <t>991015153869703851</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>management principles for health professionals</t>
+          <t>management control in nonprofit organizations</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>liebler, joan gratto.</t>
+          <t>young, david w.</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
-        <is>
-          <t>Individually Purchased eBooks</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>991017473845203851</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>management control in nonprofit organizations</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2202-20859</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sp20-NUTR-0216-01-Management Planning</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Hirsh Health Sciences Reserves</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>©2016.</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Young, David W.</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Book - Physical</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2202</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>991015153869703851</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>management control in nonprofit organizations</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>young, david w.</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
         <is>
           <t>HathiTrust (free during Covid-19)</t>
         </is>
@@ -1310,72 +1236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Course Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Course Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MMS ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Author</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>URL or Collection</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,48 +1260,163 @@
     <col width="20" customWidth="1" min="14" max="14"/>
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>MMS Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Title (Normalized)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Course Code</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Processing Department</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Author (contributor)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bibliographic Level</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Resource Type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Match MMS ID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Match Title</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Match Author</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Match Publication Year</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Match URL or Collection</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MMS Id</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Title (Normalized)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Course Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MMS ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Processing Department</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Publication Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Year</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>URL or Collection</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Author (contributor)</t>
@@ -1453,80 +1429,76 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>MMS Id</t>
+          <t>Resource Type</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Match MMS ID</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Match Title</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Match Author</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Match MMS ID</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Match Publication Year</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Match Title</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Match URL or Collection</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Processing Department</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Publication Date</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Resource Type</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Semester</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Title (Normalized)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>991005267559703851</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>focus groups a practical guide for applied research</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>2202-20857</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[2015]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Krueger, Richard A.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>Casey, Mary Anne (Mary Anne W.)</t>
@@ -1539,80 +1511,76 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>991005267559703851</t>
+          <t>Book - Physical</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>2202</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>991012436609703851</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>focus groups a practical guide for applied research</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>krueger, richard a.</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>991012436609703851</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>focus groups a practical guide for applied research</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>HathiTrust (free during Covid-19)</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Hirsh Health Sciences Reserves</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>[2015]</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Book - Physical</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>2202</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>focus groups a practical guide for applied research</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>991013153629703851</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>scale development theory and applications</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>2202-20857</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0210-01-Survey Research in Nutrition</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>c2012.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>DeVellis, Robert F.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
@@ -1621,77 +1589,77 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>991013153629703851</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
+          <t>Book - Physical</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2202</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>991001524649703851</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+          <t>991001730479703851</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>scale development theory and applications</t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>scale development theory and applications</t>
+          <t>devellis, robert f.</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>2003</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>HathiTrust (free during Covid-19)</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Hirsh Health Sciences Reserves</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>c2012.</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Book - Physical</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2202</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>scale development theory and applications</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>991017473845203851</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>management control in nonprofit organizations</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>2202-20859</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Sp20-NUTR-0216-01-Management Planning</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Liebler, Joan Gratto.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>McConnell, Charles R.</t>
-        </is>
-      </c>
+          <t>Hirsh Health Sciences Reserves</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>©2016.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Young, David W.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>m</t>
@@ -1699,139 +1667,37 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>991003181969703851</t>
+          <t>Book - Physical</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>liebler, joan gratto.</t>
+          <t>2202</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>991003081379703851</t>
+          <t>991015153869703851</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>management control in nonprofit organizations</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>management principles for health professionals</t>
+          <t>young, david w.</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Individually Purchased eBooks</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Hirsh Health Sciences Reserves</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>c2008.</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Book - Physical</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>2202</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>management principles for health professionals</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2202-20859</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Sp20-NUTR-0216-01-Management Planning</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Young, David W.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>991017473845203851</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>young, david w.</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>991015153869703851</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>management control in nonprofit organizations</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
           <t>HathiTrust (free during Covid-19)</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Hirsh Health Sciences Reserves</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>©2016.</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Book - Physical</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>2202</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>management control in nonprofit organizations</t>
         </is>
       </c>
     </row>

</xml_diff>